<commit_message>
Data para la comparacion de simulacion
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
+++ b/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t>Controlador</t>
   </si>
@@ -51,12 +51,6 @@
     <t>RTOL</t>
   </si>
   <si>
-    <t>RK</t>
-  </si>
-  <si>
-    <t>RK5</t>
-  </si>
-  <si>
     <t>PIf</t>
   </si>
   <si>
@@ -69,23 +63,98 @@
     <t>SSPRK3</t>
   </si>
   <si>
-    <t>SSPRK4</t>
-  </si>
-  <si>
-    <t>kp=0.2, 1</t>
-  </si>
-  <si>
     <t>DOPRI5(4)</t>
   </si>
   <si>
     <t>RK2</t>
+  </si>
+  <si>
+    <t>metodo</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>extra</t>
+  </si>
+  <si>
+    <t>delay = 0.5</t>
+  </si>
+  <si>
+    <t>PIf + D</t>
+  </si>
+  <si>
+    <t>PDf + I</t>
+  </si>
+  <si>
+    <t>1,1,1</t>
+  </si>
+  <si>
+    <t>delay = 2, 1,1</t>
+  </si>
+  <si>
+    <t>0.2,1,1</t>
+  </si>
+  <si>
+    <t>setpointAvz20</t>
+  </si>
+  <si>
+    <t>setpointAvz30, 0.8</t>
+  </si>
+  <si>
+    <t>setpointAvz30, 1</t>
+  </si>
+  <si>
+    <t>saturacion[0,20]</t>
+  </si>
+  <si>
+    <t>tiempoEjecucionC</t>
+  </si>
+  <si>
+    <t>tiempoEjecucionD</t>
+  </si>
+  <si>
+    <t>discreto</t>
+  </si>
+  <si>
+    <t>ZOH=0.1</t>
+  </si>
+  <si>
+    <t>tustin=0.1</t>
+  </si>
+  <si>
+    <t>tustin=0.05</t>
+  </si>
+  <si>
+    <t>backward=0.05</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>tustin=0.01</t>
+  </si>
+  <si>
+    <t>euler=0.08</t>
+  </si>
+  <si>
+    <t>impulse=0.1</t>
+  </si>
+  <si>
+    <t>ZOH=0.01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,16 +162,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,15 +216,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Énfasis2" xfId="3" builtinId="34"/>
+    <cellStyle name="40% - Énfasis1" xfId="2" builtinId="31"/>
+    <cellStyle name="40% - Énfasis2" xfId="4" builtinId="35"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,210 +575,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="10">
+        <v>1.0820724964141799</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0.50392460823059004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C3" s="1">
-        <v>1E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D3" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G3" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.82229495048522905</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0.50392484664916903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="1">
-        <v>1E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D4" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.66213417053222601</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.55666136741638095</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D5" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G5" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.67873668670654297</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D6" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="10">
+        <v>13.4243292808532</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>1</v>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D7" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G7" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="10">
+        <v>21.1472730636596</v>
+      </c>
+      <c r="I7" s="14">
+        <v>15.0640499591827</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D8" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="10">
+        <v>15.013255357742301</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C9" s="1">
         <v>9.9999999999999995E-7</v>
@@ -608,129 +834,244 @@
       <c r="D9" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G9" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="10">
+        <v>11.094165325164701</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10">
-        <v>1</v>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C10" s="1">
-        <v>1E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D10" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="E10" t="s">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="10">
+        <v>15.3394420146942</v>
+      </c>
+      <c r="I10" s="14">
+        <v>2.2071149349212602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="10">
+        <v>6.6154828071594203</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="10">
+        <v>8.9436950683593697</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="10">
+        <v>13.4174997806549</v>
+      </c>
+      <c r="I13" s="14">
+        <v>2.2149274349212602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="10">
+        <v>18.232135057449302</v>
+      </c>
+      <c r="I14" s="14">
+        <v>1.8262414932250901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D15" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="10">
+        <v>15.1734249591827</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="10">
+        <v>20.984194040298402</v>
+      </c>
+      <c r="I16" s="14">
+        <v>3.15637111663818</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G10" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D11" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G11" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D12" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D17" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G12" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D13" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G13" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G14" s="1">
-        <v>3.0000000000000001E-6</v>
+      <c r="F17" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="11">
+        <v>3.9815967082977202</v>
+      </c>
+      <c r="I17" s="17">
+        <v>6.7981116771697998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documentacion de codigo detalles
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
+++ b/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
@@ -152,7 +152,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -233,7 +233,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -256,10 +256,10 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -268,16 +268,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
@@ -289,8 +289,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30"/>
@@ -578,7 +579,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,16 +595,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="19" t="s">

</xml_diff>

<commit_message>
Data recolectada con tustin arreglado
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
+++ b/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
@@ -151,9 +151,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,7 +230,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -256,30 +253,9 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,6 +267,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -579,7 +561,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,31 +577,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -645,11 +627,11 @@
       <c r="G2" s="8">
         <v>1</v>
       </c>
-      <c r="H2" s="10">
-        <v>1.0820724964141799</v>
-      </c>
-      <c r="I2" s="12">
-        <v>0.50392460823059004</v>
+      <c r="H2" s="9">
+        <v>0.58986973762512196</v>
+      </c>
+      <c r="I2" s="9">
+        <v>0.50197410583496005</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -675,10 +657,10 @@
         <v>24</v>
       </c>
       <c r="H3" s="9">
-        <v>0.82229495048522905</v>
-      </c>
-      <c r="I3" s="12">
-        <v>0.50392484664916903</v>
+        <v>0.83108949661254805</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.53224802017211903</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -704,10 +686,10 @@
         <v>23</v>
       </c>
       <c r="H4" s="9">
-        <v>0.66213417053222601</v>
-      </c>
-      <c r="I4" s="12">
-        <v>0.55666136741638095</v>
+        <v>0.70217561721801702</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.57619571685791005</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -733,9 +715,9 @@
         <v>23</v>
       </c>
       <c r="H5" s="9">
-        <v>0.67873668670654297</v>
-      </c>
-      <c r="I5" s="13" t="s">
+        <v>0.68948197364807096</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -759,10 +741,10 @@
         <v>37</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="10">
-        <v>13.4243292808532</v>
-      </c>
-      <c r="I6" s="13" t="s">
+      <c r="H6" s="9">
+        <v>14.1812629699707</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -788,11 +770,11 @@
       <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="10">
-        <v>21.1472730636596</v>
-      </c>
-      <c r="I7" s="14">
-        <v>15.0640499591827</v>
+      <c r="H7" s="9">
+        <v>21.4208245277404</v>
+      </c>
+      <c r="I7" s="9">
+        <v>14.988908767700099</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -815,10 +797,10 @@
         <v>37</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="10">
-        <v>15.013255357742301</v>
-      </c>
-      <c r="I8" s="15" t="s">
+      <c r="H8" s="9">
+        <v>15.209624767303399</v>
+      </c>
+      <c r="I8" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -842,10 +824,10 @@
         <v>37</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="10">
-        <v>11.094165325164701</v>
-      </c>
-      <c r="I9" s="15" t="s">
+      <c r="H9" s="9">
+        <v>11.3813378810882</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -871,11 +853,11 @@
       <c r="G10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="10">
-        <v>15.3394420146942</v>
-      </c>
-      <c r="I10" s="14">
-        <v>2.2071149349212602</v>
+      <c r="H10" s="9">
+        <v>15.572923898696899</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2.2686486244201598</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -898,10 +880,10 @@
         <v>37</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="10">
-        <v>6.6154828071594203</v>
-      </c>
-      <c r="I11" s="15" t="s">
+      <c r="H11" s="9">
+        <v>6.68387603759765</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -925,10 +907,10 @@
         <v>37</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="10">
-        <v>8.9436950683593697</v>
-      </c>
-      <c r="I12" s="15" t="s">
+      <c r="H12" s="9">
+        <v>9.1830027103424001</v>
+      </c>
+      <c r="I12" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -954,11 +936,11 @@
       <c r="G13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="10">
-        <v>13.4174997806549</v>
-      </c>
-      <c r="I13" s="14">
-        <v>2.2149274349212602</v>
+      <c r="H13" s="9">
+        <v>13.751554250717099</v>
+      </c>
+      <c r="I13" s="9">
+        <v>2.10360360145568</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -983,11 +965,11 @@
       <c r="G14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="10">
-        <v>18.232135057449302</v>
-      </c>
-      <c r="I14" s="14">
-        <v>1.8262414932250901</v>
+      <c r="H14" s="9">
+        <v>18.754692316055198</v>
+      </c>
+      <c r="I14" s="9">
+        <v>1.85164093971252</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1010,10 +992,10 @@
         <v>37</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="10">
-        <v>15.1734249591827</v>
-      </c>
-      <c r="I15" s="15" t="s">
+      <c r="H15" s="9">
+        <v>15.477213382720899</v>
+      </c>
+      <c r="I15" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1039,11 +1021,11 @@
       <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="10">
-        <v>20.984194040298402</v>
-      </c>
-      <c r="I16" s="14">
-        <v>3.15637111663818</v>
+      <c r="H16" s="9">
+        <v>21.049712896347</v>
+      </c>
+      <c r="I16" s="9">
+        <v>3.2149789333343501</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1062,17 +1044,17 @@
       <c r="E17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="10" t="s">
         <v>41</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="11">
-        <v>3.9815967082977202</v>
-      </c>
-      <c r="I17" s="17">
-        <v>6.7981116771697998</v>
+      <c r="H17" s="15">
+        <v>4.2755711078643799</v>
+      </c>
+      <c r="I17" s="15">
+        <v>6.8606407642364502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comparacion simulacion continuo done, falta analisis de tiempos de ejecucion
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
+++ b/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
@@ -151,6 +151,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,9 +253,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,11 +268,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -561,7 +564,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H13" sqref="H13:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,31 +580,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -627,10 +630,10 @@
       <c r="G2" s="8">
         <v>1</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="14">
         <v>0.58986973762512196</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="14">
         <v>0.50197410583496005</v>
       </c>
     </row>
@@ -656,10 +659,10 @@
       <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="14">
         <v>0.83108949661254805</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="14">
         <v>0.53224802017211903</v>
       </c>
     </row>
@@ -685,10 +688,10 @@
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="14">
         <v>0.70217561721801702</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="14">
         <v>0.57619571685791005</v>
       </c>
     </row>
@@ -714,10 +717,10 @@
       <c r="G5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="14">
         <v>0.68948197364807096</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -741,10 +744,10 @@
         <v>37</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="9">
+      <c r="H6" s="14">
         <v>14.1812629699707</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -770,10 +773,10 @@
       <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="14">
         <v>21.4208245277404</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="14">
         <v>14.988908767700099</v>
       </c>
     </row>
@@ -797,10 +800,10 @@
         <v>37</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="9">
+      <c r="H8" s="14">
         <v>15.209624767303399</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -824,10 +827,10 @@
         <v>37</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="9">
+      <c r="H9" s="14">
         <v>11.3813378810882</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -853,10 +856,10 @@
       <c r="G10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="9">
-        <v>15.572923898696899</v>
-      </c>
-      <c r="I10" s="9">
+      <c r="H10" s="14">
+        <v>15.5729238986968</v>
+      </c>
+      <c r="I10" s="14">
         <v>2.2686486244201598</v>
       </c>
     </row>
@@ -880,10 +883,10 @@
         <v>37</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="9">
+      <c r="H11" s="14">
         <v>6.68387603759765</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -907,10 +910,10 @@
         <v>37</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="9">
+      <c r="H12" s="14">
         <v>9.1830027103424001</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -936,10 +939,10 @@
       <c r="G13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="14">
         <v>13.751554250717099</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="14">
         <v>2.10360360145568</v>
       </c>
     </row>
@@ -965,10 +968,10 @@
       <c r="G14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="14">
         <v>18.754692316055198</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="14">
         <v>1.85164093971252</v>
       </c>
     </row>
@@ -992,10 +995,10 @@
         <v>37</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="9">
+      <c r="H15" s="14">
         <v>15.477213382720899</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1021,10 +1024,10 @@
       <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="14">
         <v>21.049712896347</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="14">
         <v>3.2149789333343501</v>
       </c>
     </row>
@@ -1044,16 +1047,16 @@
       <c r="E17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="16">
         <v>4.2755711078643799</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="16">
         <v>6.8606407642364502</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corregido el orden de calculo
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
+++ b/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>Controlador</t>
   </si>
@@ -57,9 +57,6 @@
     <t>PID+f</t>
   </si>
   <si>
-    <t>ralston4</t>
-  </si>
-  <si>
     <t>SSPRK3</t>
   </si>
   <si>
@@ -145,6 +142,15 @@
   </si>
   <si>
     <t>ZOH=0.01</t>
+  </si>
+  <si>
+    <t>Fehlberg4(5)</t>
+  </si>
+  <si>
+    <t>RK4</t>
+  </si>
+  <si>
+    <t>Ralston3</t>
   </si>
 </sst>
 </file>
@@ -152,7 +158,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -268,13 +274,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -564,7 +570,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +578,7 @@
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="8" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
@@ -593,19 +599,19 @@
         <v>8</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -613,19 +619,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="D2" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
@@ -642,22 +648,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="D3" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="14">
         <v>0.83108949661254805</v>
@@ -671,22 +677,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D4" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="14">
         <v>0.70217561721801702</v>
@@ -700,28 +706,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D5" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="14">
         <v>0.68948197364807096</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -729,26 +735,26 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
-        <v>9.9999999999999995E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D6" s="1">
-        <v>9.9999999999999995E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="14">
         <v>14.1812629699707</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -756,22 +762,22 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="D7" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="14">
         <v>21.4208245277404</v>
@@ -785,26 +791,26 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
-        <v>9.9999999999999995E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D8" s="1">
-        <v>9.9999999999999995E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="14">
         <v>15.209624767303399</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -812,7 +818,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>9.9999999999999995E-7</v>
@@ -821,17 +827,17 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="14">
         <v>11.3813378810882</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -839,22 +845,22 @@
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="D10" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" s="14">
         <v>15.5729238986968</v>
@@ -868,26 +874,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1">
-        <v>9.9999999999999995E-8</v>
+        <v>1E-4</v>
       </c>
       <c r="D11" s="1">
-        <v>9.9999999999999995E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="14">
         <v>6.68387603759765</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -895,34 +901,34 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D12" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="14">
         <v>9.1830027103424001</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1">
         <v>1.0000000000000001E-5</v>
@@ -931,13 +937,13 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="14">
         <v>13.751554250717099</v>
@@ -948,25 +954,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D14" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14" s="14">
         <v>18.754692316055198</v>
@@ -980,26 +986,26 @@
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>1E-4</v>
       </c>
       <c r="D15" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="14">
         <v>15.477213382720899</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1007,7 +1013,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1">
         <v>1.0000000000000001E-5</v>
@@ -1016,13 +1022,13 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" s="14">
         <v>21.049712896347</v>
@@ -1036,7 +1042,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="6">
         <v>1.0000000000000001E-5</v>
@@ -1045,13 +1051,13 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="16">
         <v>4.2755711078643799</v>

</xml_diff>

<commit_message>
Nueva data como es
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
+++ b/comparisonFiles/Data LVSCCD/Simulacion/DataSimLV.xlsx
@@ -570,7 +570,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="14">
-        <v>0.58986973762512196</v>
+        <v>0.530292749404907</v>
       </c>
       <c r="I2" s="14">
-        <v>0.50197410583496005</v>
+        <v>0.49904227256774902</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -666,10 +666,10 @@
         <v>23</v>
       </c>
       <c r="H3" s="14">
-        <v>0.83108949661254805</v>
+        <v>0.66603994369506803</v>
       </c>
       <c r="I3" s="14">
-        <v>0.53224802017211903</v>
+        <v>0.509785175323486</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -695,10 +695,10 @@
         <v>22</v>
       </c>
       <c r="H4" s="14">
-        <v>0.70217561721801702</v>
+        <v>0.67190027236938399</v>
       </c>
       <c r="I4" s="14">
-        <v>0.57619571685791005</v>
+        <v>0.56935691833496005</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>22</v>
       </c>
       <c r="H5" s="14">
-        <v>0.68948197364807096</v>
+        <v>0.688501596450805</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>36</v>
@@ -751,7 +751,7 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="14">
-        <v>14.1812629699707</v>
+        <v>14.4302310943603</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>36</v>
@@ -780,10 +780,10 @@
         <v>25</v>
       </c>
       <c r="H7" s="14">
-        <v>21.4208245277404</v>
+        <v>10.007211923599201</v>
       </c>
       <c r="I7" s="14">
-        <v>14.988908767700099</v>
+        <v>14.7417678833007</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="14">
-        <v>15.209624767303399</v>
+        <v>13.1977627277374</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>36</v>
@@ -834,7 +834,7 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="14">
-        <v>11.3813378810882</v>
+        <v>9.8919746875762904</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>36</v>
@@ -863,10 +863,10 @@
         <v>19</v>
       </c>
       <c r="H10" s="14">
-        <v>15.5729238986968</v>
+        <v>5.9474902153015101</v>
       </c>
       <c r="I10" s="14">
-        <v>2.2686486244201598</v>
+        <v>2.2901258468627899</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="14">
-        <v>6.68387603759765</v>
+        <v>4.3761410713195801</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>36</v>
@@ -917,7 +917,7 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="14">
-        <v>9.1830027103424001</v>
+        <v>8.8802170753479004</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>36</v>
@@ -946,10 +946,10 @@
         <v>26</v>
       </c>
       <c r="H13" s="14">
-        <v>13.751554250717099</v>
+        <v>7.9954185485839799</v>
       </c>
       <c r="I13" s="14">
-        <v>2.10360360145568</v>
+        <v>2.08503866195678</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -975,10 +975,10 @@
         <v>27</v>
       </c>
       <c r="H14" s="14">
-        <v>18.754692316055198</v>
+        <v>19.328854560852001</v>
       </c>
       <c r="I14" s="14">
-        <v>1.85164093971252</v>
+        <v>1.8281934261321999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="14">
-        <v>15.477213382720899</v>
+        <v>11.078542470932</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>36</v>
@@ -1031,10 +1031,10 @@
         <v>28</v>
       </c>
       <c r="H16" s="14">
-        <v>21.049712896347</v>
+        <v>17.684261083602902</v>
       </c>
       <c r="I16" s="14">
-        <v>3.2149789333343501</v>
+        <v>3.13488340377807</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1060,10 +1060,10 @@
         <v>24</v>
       </c>
       <c r="H17" s="16">
-        <v>4.2755711078643799</v>
+        <v>4.5148169994354204</v>
       </c>
       <c r="I17" s="16">
-        <v>6.8606407642364502</v>
+        <v>6.7404875755309996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>